<commit_message>
feat: BOM Excel Import + Sample dosyası güncelleme
✅ Yeni Özellikler:
- BOM Excel import fonksiyonu eklendi
- Import butonu BOM sayfasına eklendi
- Sample Excel dosyası yeni formata uyarlandı
- Import/Export formatı birleştirildi

📊 Excel Formatı:
- Ürün Kodu, Ürün Adı, Ürün Tipi
- Malzeme Tipi, Malzeme Kodu, Malzeme Adı
- Miktar, Notlar

🔧 Import Özellikleri:
- Hem nihai hem yarı mamul ürün desteği
- Malzeme tipi validation
- Yarı mamul için sadece hammadde kontrolü
- Duplicate kayıt önleme
- Hata raporlama
- Başarı/hata istatistikleri

📁 Eklenen/Güncellenen:
- app/api/bom/import/route.ts (yeni)
- scripts/generate-bom-sample.ts (yeni)
- bom-sample-data.xlsx (güncellendi)
- public/bom-sample-data.xlsx (güncellendi)
- BOM sayfası import dialog
</commit_message>
<xml_diff>
--- a/bom-sample-data.xlsx
+++ b/bom-sample-data.xlsx
@@ -3,8 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="BOM Sample" sheetId="1" r:id="rId1"/>
-    <sheet name="Nihai Ürünler" sheetId="2" r:id="rId2"/>
+    <sheet name="BOM Listesi" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -398,311 +397,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="40.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>product_code</v>
+        <v>Ürün Kodu</v>
       </c>
       <c r="B1" t="str">
-        <v>product_name</v>
+        <v>Ürün Adı</v>
       </c>
       <c r="C1" t="str">
-        <v>material_code</v>
+        <v>Ürün Tipi</v>
       </c>
       <c r="D1" t="str">
-        <v>material_name</v>
+        <v>Malzeme Tipi</v>
       </c>
       <c r="E1" t="str">
-        <v>quantity</v>
+        <v>Malzeme Kodu</v>
       </c>
       <c r="F1" t="str">
-        <v>unit</v>
+        <v>Malzeme Adı</v>
       </c>
       <c r="G1" t="str">
-        <v>notes</v>
+        <v>Miktar</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Notlar</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>THP-001</v>
+        <v>NUP001</v>
       </c>
       <c r="B2" t="str">
-        <v>Thunder Pro Laptop</v>
+        <v>Örnek Nihai Ürün</v>
       </c>
       <c r="C2" t="str">
-        <v>CPU-001</v>
+        <v>Nihai Ürün</v>
       </c>
       <c r="D2" t="str">
-        <v>Intel Core i7 Processor</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+        <v>Hammadde</v>
+      </c>
+      <c r="E2" t="str">
+        <v>HM001</v>
       </c>
       <c r="F2" t="str">
-        <v>adet</v>
-      </c>
-      <c r="G2" t="str">
-        <v>Ana işlemci</v>
+        <v>Örnek Hammadde</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2" t="str">
+        <v>5 kg gerekli</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>THP-001</v>
+        <v>NUP001</v>
       </c>
       <c r="B3" t="str">
-        <v>Thunder Pro Laptop</v>
+        <v>Örnek Nihai Ürün</v>
       </c>
       <c r="C3" t="str">
-        <v>RAM-001</v>
+        <v>Nihai Ürün</v>
       </c>
       <c r="D3" t="str">
-        <v>DDR4 16GB RAM</v>
-      </c>
-      <c r="E3">
+        <v>Yarı Mamul</v>
+      </c>
+      <c r="E3" t="str">
+        <v>YM001</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Örnek Yarı Mamul</v>
+      </c>
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="F3" t="str">
-        <v>adet</v>
-      </c>
-      <c r="G3" t="str">
-        <v>Bellek modülü</v>
+      <c r="H3" t="str">
+        <v>2 adet yarı mamul gerekli</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>THP-001</v>
+        <v>YM001</v>
       </c>
       <c r="B4" t="str">
-        <v>Thunder Pro Laptop</v>
+        <v>Örnek Yarı Mamul</v>
       </c>
       <c r="C4" t="str">
-        <v>SSD-001</v>
+        <v>Yarı Mamul</v>
       </c>
       <c r="D4" t="str">
-        <v>512GB NVMe SSD</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
+        <v>Hammadde</v>
+      </c>
+      <c r="E4" t="str">
+        <v>HM002</v>
       </c>
       <c r="F4" t="str">
-        <v>adet</v>
-      </c>
-      <c r="G4" t="str">
-        <v>Depolama birimi</v>
+        <v>Başka Hammadde</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="str">
+        <v>3 kg gerekli</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>THP-001</v>
+        <v>YM001</v>
       </c>
       <c r="B5" t="str">
-        <v>Thunder Pro Laptop</v>
+        <v>Örnek Yarı Mamul</v>
       </c>
       <c r="C5" t="str">
-        <v>LCD-001</v>
+        <v>Yarı Mamul</v>
       </c>
       <c r="D5" t="str">
-        <v>15.6" Full HD LCD Panel</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
+        <v>Hammadde</v>
+      </c>
+      <c r="E5" t="str">
+        <v>HM003</v>
       </c>
       <c r="F5" t="str">
-        <v>adet</v>
-      </c>
-      <c r="G5" t="str">
-        <v>Ekran paneli</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>THP-001</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Thunder Pro Laptop</v>
-      </c>
-      <c r="C6" t="str">
-        <v>BAT-001</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Li-Po 5000mAh Battery</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="str">
-        <v>adet</v>
-      </c>
-      <c r="G6" t="str">
-        <v>Pil paketi</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>THP-001</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Thunder Pro Laptop</v>
-      </c>
-      <c r="C7" t="str">
-        <v>MB-001</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Ana Kart Montajı</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="str">
-        <v>adet</v>
-      </c>
-      <c r="G7" t="str">
-        <v>CPU, RAM, SSD montajlı ana kart</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>THP-001</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Thunder Pro Laptop</v>
-      </c>
-      <c r="C8" t="str">
-        <v>CH-001</v>
-      </c>
-      <c r="D8" t="str">
-        <v>Chassis Montajı</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="str">
-        <v>adet</v>
-      </c>
-      <c r="G8" t="str">
-        <v>LCD, pil, ana kart montajlı gövde</v>
+        <v>Üçüncü Hammadde</v>
+      </c>
+      <c r="G5">
+        <v>1.5</v>
+      </c>
+      <c r="H5" t="str">
+        <v>1.5 litre gerekli</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="40.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>product_code</v>
-      </c>
-      <c r="B1" t="str">
-        <v>product_name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>unit</v>
-      </c>
-      <c r="D1" t="str">
-        <v>sale_price</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>THP-001</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Thunder Pro Laptop</v>
-      </c>
-      <c r="C2" t="str">
-        <v>adet</v>
-      </c>
-      <c r="D2">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>THB-001</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Thunder Basic Laptop</v>
-      </c>
-      <c r="C3" t="str">
-        <v>adet</v>
-      </c>
-      <c r="D3">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>THM-001</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Thunder Mini Laptop</v>
-      </c>
-      <c r="C4" t="str">
-        <v>adet</v>
-      </c>
-      <c r="D4">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>THG-001</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Thunder Gaming Laptop</v>
-      </c>
-      <c r="C5" t="str">
-        <v>adet</v>
-      </c>
-      <c r="D5">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>THW-001</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Thunder Workstation</v>
-      </c>
-      <c r="C6" t="str">
-        <v>adet</v>
-      </c>
-      <c r="D6">
-        <v>45000</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: BOM notes kolonu kaldırıldı
❌ Sorun: bom tablosunda notes kolonu yok
✅ Çözüm: notes kolonu import/export'tan kaldırıldı

📊 Yeni Excel Formatı (7 kolon):
- Ürün Kodu, Ürün Adı, Ürün Tipi
- Malzeme Tipi, Malzeme Kodu, Malzeme Adı
- Miktar

🔧 Değişiklikler:
- app/api/bom/import/route.ts - notes insert kaldırıldı
- app/api/bom/export/route.ts - notes export kaldırıldı
- scripts/generate-bom-sample.ts - notes sample'dan kaldırıldı
- Sample Excel dosyaları yeniden oluşturuldu
- Kolon genişlikleri güncellendi (8→7)
</commit_message>
<xml_diff>
--- a/bom-sample-data.xlsx
+++ b/bom-sample-data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -409,7 +409,6 @@
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="30.83203125" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -434,9 +433,6 @@
       <c r="G1" t="str">
         <v>Miktar</v>
       </c>
-      <c r="H1" t="str">
-        <v>Notlar</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -460,9 +456,6 @@
       <c r="G2">
         <v>5</v>
       </c>
-      <c r="H2" t="str">
-        <v>5 kg gerekli</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -486,9 +479,6 @@
       <c r="G3">
         <v>2</v>
       </c>
-      <c r="H3" t="str">
-        <v>2 adet yarı mamul gerekli</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -512,9 +502,6 @@
       <c r="G4">
         <v>3</v>
       </c>
-      <c r="H4" t="str">
-        <v>3 kg gerekli</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -538,13 +525,10 @@
       <c r="G5">
         <v>1.5</v>
       </c>
-      <c r="H5" t="str">
-        <v>1.5 litre gerekli</v>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>